<commit_message>
this is chanegs to read the excel file
</commit_message>
<xml_diff>
--- a/Maven/TestData/TestData.xlsx
+++ b/Maven/TestData/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WORK\git\WebApps\Maven\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A7591A-82C3-4EAA-90C4-7250A79E1487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399F3C0B-23FF-48FE-9441-76F913E5A6D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="SearchAddCustomer" sheetId="2" r:id="rId2"/>
+    <sheet name="NewCustomer" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>vijaytest@gnrgy</t>
   </si>
@@ -35,6 +36,24 @@
   </si>
   <si>
     <t>vijay</t>
+  </si>
+  <si>
+    <t>Adithya</t>
+  </si>
+  <si>
+    <t>athreya</t>
+  </si>
+  <si>
+    <t>bengaluru</t>
+  </si>
+  <si>
+    <t>srinivasa nagar</t>
+  </si>
+  <si>
+    <t>adithya.athreya@gmail.com</t>
+  </si>
+  <si>
+    <t>This is first customer in POM</t>
   </si>
 </sst>
 </file>
@@ -395,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB8A55E-EAC1-41D5-A936-EFB1602B1C0B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -409,4 +428,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE55D2E-2702-4924-8C31-D6D8CC6FF94F}">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1">
+        <v>131</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1">
+        <v>9742315935</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F1" r:id="rId1" xr:uid="{F197213E-8379-430B-B4EC-05351B0478C0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commit entire project last changed is Country code
</commit_message>
<xml_diff>
--- a/Maven/TestData/TestData.xlsx
+++ b/Maven/TestData/TestData.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WORK\git\WebApps\Maven\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399F3C0B-23FF-48FE-9441-76F913E5A6D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9506996-2E93-47B0-BA33-F51C1F647474}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5520" yWindow="0" windowWidth="23280" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="SearchAddCustomer" sheetId="2" r:id="rId2"/>
+    <sheet name="SearchCustomer" sheetId="2" r:id="rId2"/>
     <sheet name="NewCustomer" sheetId="3" r:id="rId3"/>
+    <sheet name="Twitter" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,40 +28,76 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>vijaytest@gnrgy</t>
   </si>
   <si>
+    <t>Adithya</t>
+  </si>
+  <si>
+    <t>athreya</t>
+  </si>
+  <si>
+    <t>bengaluru</t>
+  </si>
+  <si>
+    <t>srinivasa nagar</t>
+  </si>
+  <si>
+    <t>adithya.athreya@gmail.com</t>
+  </si>
+  <si>
+    <t>This is first customer in POM</t>
+  </si>
+  <si>
+    <t>Please enter the first name</t>
+  </si>
+  <si>
+    <t>Please enter the last name</t>
+  </si>
+  <si>
+    <t>Please enter the city name</t>
+  </si>
+  <si>
+    <t>Please enter the street name</t>
+  </si>
+  <si>
+    <t>Please enter the house number</t>
+  </si>
+  <si>
+    <t>Please enter the mobile number</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>9742315935</t>
+  </si>
+  <si>
+    <t>adithya</t>
+  </si>
+  <si>
+    <t>vijayakrishna10896@gmail.com</t>
+  </si>
+  <si>
+    <t>Mukhyaprana@10</t>
+  </si>
+  <si>
     <t>abc@123</t>
   </si>
   <si>
-    <t>vijay</t>
-  </si>
-  <si>
-    <t>Adithya</t>
-  </si>
-  <si>
-    <t>athreya</t>
-  </si>
-  <si>
-    <t>bengaluru</t>
-  </si>
-  <si>
-    <t>srinivasa nagar</t>
-  </si>
-  <si>
-    <t>adithya.athreya@gmail.com</t>
-  </si>
-  <si>
-    <t>This is first customer in POM</t>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>+91</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +109,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,9 +142,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -385,7 +431,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,7 +444,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -414,15 +460,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB8A55E-EAC1-41D5-A936-EFB1602B1C0B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -432,10 +476,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE55D2E-2702-4924-8C31-D6D8CC6FF94F}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,32 +489,69 @@
     <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="E1">
-        <v>131</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="G1">
-        <v>9742315935</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -478,5 +559,37 @@
     <hyperlink ref="F1" r:id="rId1" xr:uid="{F197213E-8379-430B-B4EC-05351B0478C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE1AAA2-1DCF-4A06-9786-F7B888B12DF7}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{2CCD0D95-C205-477B-B56E-59B7FEFEF8E4}"/>
+    <hyperlink ref="B1" r:id="rId2" xr:uid="{6DFB37ED-D821-402A-82E3-0CE94FDEE8DE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>